<commit_message>
Liste erweitert und neu Gruppierung in Lösungen/Packages
</commit_message>
<xml_diff>
--- a/tools.xlsx
+++ b/tools.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vepo\Documents\GitRepo\operationalisierung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soga\Documents\02_Projekte\00_Operationalisierung\operationalisierung\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="13248"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="13245"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
   <si>
     <t>Name</t>
   </si>
@@ -122,18 +122,12 @@
     <t>sparklyr</t>
   </si>
   <si>
-    <t>dplyr back-end</t>
-  </si>
-  <si>
     <t>Microsoft DeployR</t>
   </si>
   <si>
     <t xml:space="preserve">Microsoft R Server (Microsoft Machine Learning Server) /SQL Server </t>
   </si>
   <si>
-    <t>ähnlich wie Plumber, whl veraltet</t>
-  </si>
-  <si>
     <t>Serialisierung (ist R Package)</t>
   </si>
   <si>
@@ -158,12 +152,6 @@
     <t>NUR mit Kreditkarte möglich</t>
   </si>
   <si>
-    <t>DeployR open ist frei zugänglich, es muss aber MS machine Learning Server installiert sein)</t>
-  </si>
-  <si>
-    <t>https://docs.microsoft.com/en-us/machine-learning-server/operationalize/concept-what-are-web-services, https://docs.microsoft.com/en-us/machine-learning-server/deployr/deployr-about</t>
-  </si>
-  <si>
     <t>knowru</t>
   </si>
   <si>
@@ -177,13 +165,103 @@
   </si>
   <si>
     <t>Für Windows über VMWare (virtuelle Maschine, private Nutzung), um Ubuntu zu integrieren</t>
+  </si>
+  <si>
+    <t>Vorschläge von plumber-Dokumentation (Chapter 7: Hosting)</t>
+  </si>
+  <si>
+    <t>https://www.rplumber.io/docs/hosting.html#pm2</t>
+  </si>
+  <si>
+    <t>DigitalOcean</t>
+  </si>
+  <si>
+    <t>Docker</t>
+  </si>
+  <si>
+    <t>Rstudio Connect (siehe oben)</t>
+  </si>
+  <si>
+    <t>Docker provides a way to run applications securely isolated in a container, packaged with all its dependencies and libraries. https://docs.docker.com/</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>free 10$ credit</t>
+  </si>
+  <si>
+    <t>verschiedene Modelle, von 5$ - 80$ pro Monat</t>
+  </si>
+  <si>
+    <t>process manager to set up a server that automatically starts your plumber services when booted, restarts them if they ever crash, and even centralizes the logs for your plumber services. (probably not what we need since we have Devs)</t>
+  </si>
+  <si>
+    <t>Cloud computing, designed for developpers: DigitalOcean is an easy-to-use Cloud Computing provider. They offer a simple way to spin up a Linux virtual machine and access it remotely.  https://www.digitalocean.com/</t>
+  </si>
+  <si>
+    <t>plumber kann verwendet werden, siehe: https://blog.rstudio.com/2017/08/03/rstudio-connect-v1-5-4-plumber/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hilfreiche Packages </t>
+  </si>
+  <si>
+    <t>Mögliche Lösungen  für Operationalisierung</t>
+  </si>
+  <si>
+    <t>z.B. um APIs zu kreieren</t>
+  </si>
+  <si>
+    <t>jug</t>
+  </si>
+  <si>
+    <t>(pm2)</t>
+  </si>
+  <si>
+    <t>Jug is a small web development framework for R which relies heavily upon the httpuv package. It’s main focus is to make building APIs for your code as easy as possible. Pipe operator http://bart6114.github.io/jug/articles/jug.html</t>
+  </si>
+  <si>
+    <t>SparkR</t>
+  </si>
+  <si>
+    <t>SparkR vs. Sparklyr : https://stackoverflow.com/questions/39494484/sparkr-vs-sparklyr</t>
+  </si>
+  <si>
+    <t>SparkR is an R package that provides a light-weight frontend to use Apache Spark from R.</t>
+  </si>
+  <si>
+    <t>plumber allows you to create a REST API by decorating your existing R source code with special comments. https://www.rplumber.io/docs/index.html</t>
+  </si>
+  <si>
+    <t>Connect from R to Spark.</t>
+  </si>
+  <si>
+    <t>DeployR Open ist frei zugänglich, es muss aber MS machine Learning Server installiert sein)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DeployR Open is an open-source server-based framework for R, that makes it easy to call out to the server to run R code in real time. https://docs.microsoft.com/en-us/machine-learning-server/operationalize/concept-what-are-web-services, https://docs.microsoft.com/en-us/machine-learning-server/deployr/deployr-about </t>
+  </si>
+  <si>
+    <t>http://blog.revolutionanalytics.com/2014/10/integrate-r-into-applications-with-deployr-open.html</t>
+  </si>
+  <si>
+    <t>weitere Kommentare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCP/IP server </t>
+  </si>
+  <si>
+    <t>möglicherweise veraltet. Rserve is a TCP/IP server which allows other programs to use facilities of R (see www.r-project.org) from various languages without the need to initialize R or link against R library. Every connection has a separate workspace and working directory. Client-side implementations are available for popular languages such as C/C++, PHP and Java. Rserve supports remote connection, authentication and file transfer. Typical use is to integrate R backend for computation of statstical models, plots etc. in other applications.  https://www.rforge.net/Rserve/</t>
+  </si>
+  <si>
+    <t>Es gibt auch noch ein Rserve R-package</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -196,6 +274,33 @@
       <color theme="4"/>
       <name val="AA Zuehlke"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="AA Zuehlke"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="AA Zuehlke"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="4"/>
+      <name val="AA Zuehlke"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="4"/>
+      <name val="AA Zuehlke"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -222,10 +327,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -238,8 +344,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -526,173 +643,183 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="3" width="24.6640625" customWidth="1"/>
-    <col min="6" max="6" width="44.109375" customWidth="1"/>
-    <col min="7" max="7" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" customWidth="1"/>
+    <col min="2" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="45.5703125" customWidth="1"/>
+    <col min="7" max="7" width="55.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="92.4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" ht="92.4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="G7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -700,13 +827,10 @@
       <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -714,19 +838,13 @@
       <c r="C10" t="s">
         <v>10</v>
       </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -737,16 +855,16 @@
       <c r="D11" t="s">
         <v>10</v>
       </c>
-      <c r="E11" t="s">
-        <v>29</v>
+      <c r="F11" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>25</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -758,80 +876,184 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    </row>
+    <row r="14" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>31</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B33" t="s">
         <v>20</v>
       </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="G33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" t="s">
         <v>20</v>
       </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>40</v>
+      <c r="G34" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C22" r:id="rId1" location="pm2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="58" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MS Azure ML updated
</commit_message>
<xml_diff>
--- a/tools.xlsx
+++ b/tools.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -129,9 +129,6 @@
   </si>
   <si>
     <t>Sehr technisch (kreiert alles über packages), und am Ende muss Kunde eingeben wie Output aussehen soll</t>
-  </si>
-  <si>
-    <t>Man muss in MS Azure den Code nochmals strukturieren und eingeben.</t>
   </si>
   <si>
     <t>NUR mit Kreditkarte möglich</t>
@@ -310,6 +307,15 @@
   </si>
   <si>
     <t>Dauer Gratisversion</t>
+  </si>
+  <si>
+    <t>Ja, erhältlich unter https://studio.azureml.net/</t>
+  </si>
+  <si>
+    <t>Drag and Drop Tool für ML, nicht gedacht um R-Skripte zu schreiben. Man kann zwar auch R-Skripte reinladen, aber dafür ist es wohl eher nicht gedacht. Man muss in MS Azure den Code nochmals strukturieren und eingeben.</t>
+  </si>
+  <si>
+    <t>Commercial Tool for doing machine learning and operationalize your solution</t>
   </si>
 </sst>
 </file>
@@ -717,7 +723,7 @@
   <dimension ref="A1:L195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -735,7 +741,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -753,49 +759,49 @@
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>24</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -803,7 +809,7 @@
     </row>
     <row r="4" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -824,14 +830,14 @@
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -857,7 +863,7 @@
         <v>9</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -880,7 +886,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -888,7 +894,7 @@
         <v>34</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -898,7 +904,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>8</v>
@@ -906,13 +912,13 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -964,14 +970,17 @@
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="G11" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="I11" s="1" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -994,7 +1003,7 @@
         <v>25</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1022,7 +1031,7 @@
     </row>
     <row r="14" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
@@ -1031,7 +1040,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="I14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1125,11 +1134,11 @@
     </row>
     <row r="22" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1139,24 +1148,24 @@
     </row>
     <row r="23" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -1164,7 +1173,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1176,17 +1185,17 @@
     </row>
     <row r="25" spans="1:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="G25" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -1194,17 +1203,17 @@
     </row>
     <row r="26" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="G26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -1242,10 +1251,10 @@
     </row>
     <row r="30" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1265,10 +1274,10 @@
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="G31" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -1276,7 +1285,7 @@
     </row>
     <row r="32" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>17</v>
@@ -1285,10 +1294,10 @@
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="H32" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -1307,10 +1316,10 @@
       </c>
       <c r="E33" s="1"/>
       <c r="G33" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -1318,7 +1327,7 @@
     </row>
     <row r="34" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>17</v>
@@ -1327,7 +1336,7 @@
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="G34" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>

</xml_diff>

<commit_message>
Zusatzinfo zu MS R Server
</commit_message>
<xml_diff>
--- a/tools.xlsx
+++ b/tools.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="90">
   <si>
     <t>Name</t>
   </si>
@@ -297,9 +297,6 @@
     <t>Ja, Open Source Version DeployR Open ist frei zugänglich, es muss aber ein Server existieren, auf dem MS machine Learning Server installiert ist</t>
   </si>
   <si>
-    <t>Namen ist verwirrend: MS R Server ist kein Server, sondern ein Framework, um auf einem (bestehenden) Server oder auf einer Cloud (z.B. von MS Azure) R-Skripte laufen zu lassen. Beinhaltet R-distribution (MS R Open), welche bestimmte MS packages enthält, welche Deployment und Parallelisierung auf Server oder Cloud, auf welcher MS R Server installiert ist, zulassen. (mrsdeploy, RevoScaleR)</t>
-  </si>
-  <si>
     <t>Preis</t>
   </si>
   <si>
@@ -316,6 +313,14 @@
   </si>
   <si>
     <t>Commercial Tool for doing machine learning and operationalize your solution</t>
+  </si>
+  <si>
+    <t>Namen ist verwirrend: MS R Server ist kein Server, sondern ein Framework, um auf einem (bestehenden) Server oder auf einer Cloud (z.B. von MS Azure) R-Skripte laufen zu lassen. Beinhaltet R-distribution (MS R Open), welche bestimmte MS packages enthält, welche Deployment und Parallelisierung auf Server oder Cloud, auf welcher MS R Server installiert ist, zulassen. (mrsdeploy, RevoScaleR)
+R and Python code and models can be deployed as web services. Exposed as web services hosted in Machine Learning Server, these models and code can be accessed and consumed in R, Python, programmatically using REST APIs, or using Swagger generated client libraries. Web services can be deployed from one platform and consumed on another. They can be consumed synchronously, in realtime, or in batch mode.</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/machine-learning-server/
+https://docs.microsoft.com/en-us/machine-learning-server/operationalize/concept-what-are-web-services</t>
   </si>
 </sst>
 </file>
@@ -399,16 +404,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -419,14 +421,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -723,7 +731,7 @@
   <dimension ref="A1:L195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -739,14 +747,14 @@
     <col min="10" max="10" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:12" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -759,13 +767,13 @@
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>66</v>
@@ -780,692 +788,833 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:12" ht="155.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="8"/>
+      <c r="F3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="G3" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="8"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="G5" s="4" t="s">
+      <c r="E5" s="9"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="J5" s="1"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="1"/>
+      <c r="J6" s="8"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4" t="s">
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="9" t="s">
         <v>40</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="G8" s="1" t="s">
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="J8" s="1"/>
+      <c r="J8" s="8"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="I10" s="1" t="s">
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="1"/>
+      <c r="J10" s="8"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J11" s="1"/>
+      <c r="J11" s="8"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="1"/>
+      <c r="J12" s="8"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="1"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="I14" s="1" t="s">
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="1"/>
+      <c r="J14" s="8"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1" t="s">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J15" s="1"/>
+      <c r="J15" s="8"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="I16" s="1" t="s">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="J16" s="1"/>
+      <c r="J16" s="8"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="J18" s="1"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="J19" s="1"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="J20" s="1"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="J21" s="1"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="9" t="s">
+      <c r="B22" s="8"/>
+      <c r="C22" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="J22" s="1"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1" t="s">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="H23" s="9" t="s">
+      <c r="H23" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="J23" s="1"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="J24" s="1"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="G25" s="5" t="s">
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="H25" s="9" t="s">
+      <c r="H25" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="J25" s="1"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="G26" s="1" t="s">
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="H26" s="8"/>
+      <c r="I26" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="J26" s="1"/>
+      <c r="J26" s="8"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="J27" s="1"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="J28" s="1"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="J29" s="1"/>
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="11" t="s">
+    <row r="30" spans="1:12" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="J30" s="1"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="G31" s="1" t="s">
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="H31" s="9" t="s">
+      <c r="H31" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="J31" s="1"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="H32" s="9" t="s">
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="I32" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="J32" s="1"/>
+      <c r="J32" s="8"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1" t="s">
+      <c r="C33" s="8"/>
+      <c r="D33" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="1"/>
-      <c r="G33" s="1" t="s">
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="H33" s="8"/>
+      <c r="I33" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="J33" s="1"/>
+      <c r="J33" s="8"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="G34" s="1" t="s">
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="J34" s="1"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
     <row r="35" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="H35" s="9" t="s">
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J35" s="1"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="J36" s="1"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="J37" s="1"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="J38" s="1"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="J39" s="1"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="J40" s="1"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="J41" s="1"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="J42" s="1"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="J43" s="1"/>
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="J44" s="1"/>
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="J45" s="1"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="J46" s="1"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
     </row>

</xml_diff>

<commit_message>
Upload OpenCPU.docx and modified tools.xlsx
</commit_message>
<xml_diff>
--- a/tools.xlsx
+++ b/tools.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soga\Documents\02_Projekte\00_Operationalisierung\operationalisierung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vepo\Documents\GitRepo\operationalisierung\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="13245"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="13248"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="102">
   <si>
     <t>Name</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Ja</t>
   </si>
   <si>
-    <t>Base - $14,995 per year, Standard - $24,995 per year</t>
-  </si>
-  <si>
     <t>Verbindung mit R</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t>whl veraltet</t>
   </si>
   <si>
-    <t>Sehr technisch (kreiert alles über packages), und am Ende muss Kunde eingeben wie Output aussehen soll</t>
-  </si>
-  <si>
     <t>NUR mit Kreditkarte möglich</t>
   </si>
   <si>
@@ -140,15 +134,9 @@
     <t>nur R und Python, Nutzerkonto muss angelegt werden</t>
   </si>
   <si>
-    <t>frei zugänglich, braucht Ubuntu 16.04</t>
-  </si>
-  <si>
     <t>Installation</t>
   </si>
   <si>
-    <t>Für Windows über VMWare (virtuelle Maschine, private Nutzung), um Ubuntu zu integrieren</t>
-  </si>
-  <si>
     <t>Vorschläge von plumber-Dokumentation (Chapter 7: Hosting)</t>
   </si>
   <si>
@@ -171,9 +159,6 @@
   </si>
   <si>
     <t>verschiedene Modelle, von 5$ - 80$ pro Monat</t>
-  </si>
-  <si>
-    <t>plumber kann verwendet werden, siehe: https://blog.rstudio.com/2017/08/03/rstudio-connect-v1-5-4-plumber/</t>
   </si>
   <si>
     <t xml:space="preserve">Hilfreiche Packages </t>
@@ -321,6 +306,59 @@
   <si>
     <t>https://docs.microsoft.com/en-us/machine-learning-server/
 https://docs.microsoft.com/en-us/machine-learning-server/operationalize/concept-what-are-web-services</t>
+  </si>
+  <si>
+    <t>frei zugänglich, braucht Ubuntu 16.04 oder höher</t>
+  </si>
+  <si>
+    <t>Ja, es muss aber für OpenCPU Server eine IP Adresse schon vorhanden sein</t>
+  </si>
+  <si>
+    <t>OpenCPU kann sowohl über localhost als auch einen Server agieren. Local wird ein R-Package erstellt und dieses als App gestartet. Dabei läuft R die ganze Zeit und kann keine Berechnungen ausführen. Über Postman kann man dann die API abrufen, wobei man einen extra Link als Ergebnis erhält, den man wiederum ausführen muss, um das gewünschte Ergebnis zu erhalten. Als Server ist OpenCPU ein Framework, welches einen bestehenden Server (IP Adresse) benötigt.</t>
+  </si>
+  <si>
+    <t>Da Ubuntu 16.04 oder höher benötigt wird, muss für Windows über VMWare (virtuelle Maschine, private Nutzung) installiert werden, um Ubuntu zu integrieren.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commerical Tool </t>
+  </si>
+  <si>
+    <t>free available</t>
+  </si>
+  <si>
+    <t>Verbindung zwischen R und Spark.</t>
+  </si>
+  <si>
+    <t>RStudio Connect is a new publishing platform for the work your teams create in R. Share Shiny applications, R Markdown reports, dashboards, plots, and more in one convenient place. Use push-button publishing from the RStudio IDE, scheduled execution of reports, and flexible security policies to bring the power of data science to your entire enterprise.</t>
+  </si>
+  <si>
+    <t>https://www.rstudio.com/products/connect/</t>
+  </si>
+  <si>
+    <t>plumber kann verwendet werden, siehe: https://blog.rstudio.com/2017/08/03/rstudio-connect-v1-5-4-plumber/
+Um R Funktionen als REST APIs zu nutzen, muss "Standard" oder besser verwendet werden.</t>
+  </si>
+  <si>
+    <t>Base - $14,995 per year, Standard - $24,995 per year, Enterprise - $74,995 per year</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Für loacalhost (mit Postman) einfach handhabbar. Benötigt aber Tools wie DigitalOcean, Rstudio Connect, Docker etc. um auch API über Web Server zu kreieren.</t>
+  </si>
+  <si>
+    <t>https://www.opencpu.org/ 
+Dokumentation: https://opencpu.github.io/server-manual/opencpu-server.pdf</t>
+  </si>
+  <si>
+    <t>Als Server benötigt plumber Tools wie DigitalOcean, Rstudio Connect, Docker etc.</t>
+  </si>
+  <si>
+    <t>Kann für Desktop (Windows, Mac) als auch für Server als auch Cloud Providers heruntergeladen werden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mehr ein Speichersystem. Es ist möglich über eine Docker Machine eine API Adresse mit Container zu kreieren. Dies benötigt aber Zugang zu anderem Tool z.B. DigitalOcean (siehe https://www.youtube.com/watch?v=jlVrYgVEl6M) </t>
   </si>
 </sst>
 </file>
@@ -377,18 +415,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -404,7 +436,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -424,9 +456,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -436,6 +465,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -731,32 +767,33 @@
   <dimension ref="A1:L195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="45.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="37.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" style="1" customWidth="1"/>
+    <col min="7" max="8" width="45.5546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="37.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -764,63 +801,63 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="155.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -834,33 +871,33 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="9" t="s">
+    <row r="5" spans="1:12" s="14" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="8" t="s">
+      <c r="D5" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+    </row>
+    <row r="6" spans="1:12" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
@@ -874,56 +911,62 @@
         <v>8</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+        <v>95</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>93</v>
+      </c>
       <c r="I6" s="8" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:12" s="14" customFormat="1" ht="118.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+    </row>
+    <row r="8" spans="1:12" ht="95.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>8</v>
@@ -932,21 +975,21 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>65</v>
+        <v>57</v>
+      </c>
+      <c r="H8" t="s">
+        <v>60</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>7</v>
@@ -964,7 +1007,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>6</v>
       </c>
@@ -980,15 +1023,15 @@
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="66" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>7</v>
@@ -997,26 +1040,26 @@
         <v>8</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>7</v>
@@ -1028,21 +1071,21 @@
         <v>8</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>7</v>
@@ -1054,19 +1097,21 @@
         <v>8</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="G13" s="8" t="s">
+        <v>91</v>
+      </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
@@ -1078,15 +1123,15 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
@@ -1096,21 +1141,21 @@
         <v>8</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1120,13 +1165,13 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J16" s="8"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1140,7 +1185,7 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -1154,7 +1199,7 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -1168,7 +1213,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -1182,7 +1227,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1196,13 +1241,13 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
-        <v>41</v>
+    <row r="22" spans="1:12" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="B22" s="8"/>
-      <c r="C22" s="10" t="s">
-        <v>42</v>
+      <c r="C22" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -1214,35 +1259,37 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="8"/>
+        <v>39</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H23" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -1256,29 +1303,39 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
+      <c r="D25" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>96</v>
+      </c>
       <c r="G25" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
+        <v>62</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1286,17 +1343,17 @@
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="8" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -1310,7 +1367,7 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -1324,7 +1381,7 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -1338,12 +1395,12 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="12" t="s">
-        <v>50</v>
+    <row r="30" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -1356,87 +1413,99 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
+        <v>67</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>99</v>
+      </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="10" t="s">
-        <v>74</v>
+      <c r="H32" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="J32" s="8"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="D33" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="H33" s="8"/>
       <c r="I33" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="J33" s="8"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
@@ -1444,27 +1513,29 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
-    <row r="35" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" s="8"/>
+        <v>28</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
-      <c r="H35" s="10" t="s">
-        <v>31</v>
+      <c r="H35" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -1478,7 +1549,7 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -1492,7 +1563,7 @@
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -1506,7 +1577,7 @@
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -1520,7 +1591,7 @@
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -1534,7 +1605,7 @@
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -1548,7 +1619,7 @@
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -1562,7 +1633,7 @@
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -1576,7 +1647,7 @@
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -1590,7 +1661,7 @@
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -1604,7 +1675,7 @@
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -1618,7 +1689,7 @@
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1628,7 +1699,7 @@
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1638,7 +1709,7 @@
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1648,7 +1719,7 @@
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1658,7 +1729,7 @@
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1668,7 +1739,7 @@
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1678,7 +1749,7 @@
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1688,7 +1759,7 @@
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1698,7 +1769,7 @@
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1708,7 +1779,7 @@
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1718,7 +1789,7 @@
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1728,7 +1799,7 @@
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1738,7 +1809,7 @@
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1748,7 +1819,7 @@
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1758,7 +1829,7 @@
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1768,7 +1839,7 @@
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1778,7 +1849,7 @@
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1788,7 +1859,7 @@
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1798,7 +1869,7 @@
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1808,7 +1879,7 @@
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1818,7 +1889,7 @@
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1828,7 +1899,7 @@
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1838,7 +1909,7 @@
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1848,7 +1919,7 @@
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1858,7 +1929,7 @@
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1868,7 +1939,7 @@
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1878,7 +1949,7 @@
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1888,7 +1959,7 @@
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1898,7 +1969,7 @@
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1908,7 +1979,7 @@
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1918,7 +1989,7 @@
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1928,7 +1999,7 @@
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1938,7 +2009,7 @@
       <c r="K78" s="1"/>
       <c r="L78" s="1"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -1948,7 +2019,7 @@
       <c r="K79" s="1"/>
       <c r="L79" s="1"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -1958,7 +2029,7 @@
       <c r="K80" s="1"/>
       <c r="L80" s="1"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -1968,7 +2039,7 @@
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -1978,7 +2049,7 @@
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -1988,7 +2059,7 @@
       <c r="K83" s="1"/>
       <c r="L83" s="1"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -1998,7 +2069,7 @@
       <c r="K84" s="1"/>
       <c r="L84" s="1"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2008,7 +2079,7 @@
       <c r="K85" s="1"/>
       <c r="L85" s="1"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2018,7 +2089,7 @@
       <c r="K86" s="1"/>
       <c r="L86" s="1"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2028,7 +2099,7 @@
       <c r="K87" s="1"/>
       <c r="L87" s="1"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2038,7 +2109,7 @@
       <c r="K88" s="1"/>
       <c r="L88" s="1"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2048,7 +2119,7 @@
       <c r="K89" s="1"/>
       <c r="L89" s="1"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2058,7 +2129,7 @@
       <c r="K90" s="1"/>
       <c r="L90" s="1"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2068,7 +2139,7 @@
       <c r="K91" s="1"/>
       <c r="L91" s="1"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2078,7 +2149,7 @@
       <c r="K92" s="1"/>
       <c r="L92" s="1"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2088,7 +2159,7 @@
       <c r="K93" s="1"/>
       <c r="L93" s="1"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2098,7 +2169,7 @@
       <c r="K94" s="1"/>
       <c r="L94" s="1"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2108,7 +2179,7 @@
       <c r="K95" s="1"/>
       <c r="L95" s="1"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2118,7 +2189,7 @@
       <c r="K96" s="1"/>
       <c r="L96" s="1"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2128,7 +2199,7 @@
       <c r="K97" s="1"/>
       <c r="L97" s="1"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2138,7 +2209,7 @@
       <c r="K98" s="1"/>
       <c r="L98" s="1"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2148,7 +2219,7 @@
       <c r="K99" s="1"/>
       <c r="L99" s="1"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2158,7 +2229,7 @@
       <c r="K100" s="1"/>
       <c r="L100" s="1"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -2168,7 +2239,7 @@
       <c r="K101" s="1"/>
       <c r="L101" s="1"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -2178,7 +2249,7 @@
       <c r="K102" s="1"/>
       <c r="L102" s="1"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2188,7 +2259,7 @@
       <c r="K103" s="1"/>
       <c r="L103" s="1"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -2198,7 +2269,7 @@
       <c r="K104" s="1"/>
       <c r="L104" s="1"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2208,7 +2279,7 @@
       <c r="K105" s="1"/>
       <c r="L105" s="1"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2218,7 +2289,7 @@
       <c r="K106" s="1"/>
       <c r="L106" s="1"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -2228,7 +2299,7 @@
       <c r="K107" s="1"/>
       <c r="L107" s="1"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -2238,7 +2309,7 @@
       <c r="K108" s="1"/>
       <c r="L108" s="1"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -2248,7 +2319,7 @@
       <c r="K109" s="1"/>
       <c r="L109" s="1"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -2258,7 +2329,7 @@
       <c r="K110" s="1"/>
       <c r="L110" s="1"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -2268,7 +2339,7 @@
       <c r="K111" s="1"/>
       <c r="L111" s="1"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -2278,7 +2349,7 @@
       <c r="K112" s="1"/>
       <c r="L112" s="1"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -2288,7 +2359,7 @@
       <c r="K113" s="1"/>
       <c r="L113" s="1"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -2298,7 +2369,7 @@
       <c r="K114" s="1"/>
       <c r="L114" s="1"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -2308,7 +2379,7 @@
       <c r="K115" s="1"/>
       <c r="L115" s="1"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -2318,7 +2389,7 @@
       <c r="K116" s="1"/>
       <c r="L116" s="1"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -2328,7 +2399,7 @@
       <c r="K117" s="1"/>
       <c r="L117" s="1"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -2338,7 +2409,7 @@
       <c r="K118" s="1"/>
       <c r="L118" s="1"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -2348,7 +2419,7 @@
       <c r="K119" s="1"/>
       <c r="L119" s="1"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -2358,7 +2429,7 @@
       <c r="K120" s="1"/>
       <c r="L120" s="1"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -2368,7 +2439,7 @@
       <c r="K121" s="1"/>
       <c r="L121" s="1"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -2378,7 +2449,7 @@
       <c r="K122" s="1"/>
       <c r="L122" s="1"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -2388,7 +2459,7 @@
       <c r="K123" s="1"/>
       <c r="L123" s="1"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -2398,7 +2469,7 @@
       <c r="K124" s="1"/>
       <c r="L124" s="1"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -2408,7 +2479,7 @@
       <c r="K125" s="1"/>
       <c r="L125" s="1"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -2418,7 +2489,7 @@
       <c r="K126" s="1"/>
       <c r="L126" s="1"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -2428,7 +2499,7 @@
       <c r="K127" s="1"/>
       <c r="L127" s="1"/>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -2438,7 +2509,7 @@
       <c r="K128" s="1"/>
       <c r="L128" s="1"/>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -2448,7 +2519,7 @@
       <c r="K129" s="1"/>
       <c r="L129" s="1"/>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -2458,7 +2529,7 @@
       <c r="K130" s="1"/>
       <c r="L130" s="1"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -2468,7 +2539,7 @@
       <c r="K131" s="1"/>
       <c r="L131" s="1"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -2478,7 +2549,7 @@
       <c r="K132" s="1"/>
       <c r="L132" s="1"/>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -2488,7 +2559,7 @@
       <c r="K133" s="1"/>
       <c r="L133" s="1"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -2498,7 +2569,7 @@
       <c r="K134" s="1"/>
       <c r="L134" s="1"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -2508,7 +2579,7 @@
       <c r="K135" s="1"/>
       <c r="L135" s="1"/>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -2518,7 +2589,7 @@
       <c r="K136" s="1"/>
       <c r="L136" s="1"/>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -2528,7 +2599,7 @@
       <c r="K137" s="1"/>
       <c r="L137" s="1"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -2538,7 +2609,7 @@
       <c r="K138" s="1"/>
       <c r="L138" s="1"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -2548,7 +2619,7 @@
       <c r="K139" s="1"/>
       <c r="L139" s="1"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -2558,7 +2629,7 @@
       <c r="K140" s="1"/>
       <c r="L140" s="1"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -2568,7 +2639,7 @@
       <c r="K141" s="1"/>
       <c r="L141" s="1"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -2578,7 +2649,7 @@
       <c r="K142" s="1"/>
       <c r="L142" s="1"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -2588,7 +2659,7 @@
       <c r="K143" s="1"/>
       <c r="L143" s="1"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -2598,7 +2669,7 @@
       <c r="K144" s="1"/>
       <c r="L144" s="1"/>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -2608,7 +2679,7 @@
       <c r="K145" s="1"/>
       <c r="L145" s="1"/>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -2618,7 +2689,7 @@
       <c r="K146" s="1"/>
       <c r="L146" s="1"/>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -2628,7 +2699,7 @@
       <c r="K147" s="1"/>
       <c r="L147" s="1"/>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -2638,7 +2709,7 @@
       <c r="K148" s="1"/>
       <c r="L148" s="1"/>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -2648,7 +2719,7 @@
       <c r="K149" s="1"/>
       <c r="L149" s="1"/>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -2658,7 +2729,7 @@
       <c r="K150" s="1"/>
       <c r="L150" s="1"/>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -2668,7 +2739,7 @@
       <c r="K151" s="1"/>
       <c r="L151" s="1"/>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -2678,7 +2749,7 @@
       <c r="K152" s="1"/>
       <c r="L152" s="1"/>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -2688,7 +2759,7 @@
       <c r="K153" s="1"/>
       <c r="L153" s="1"/>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -2698,7 +2769,7 @@
       <c r="K154" s="1"/>
       <c r="L154" s="1"/>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -2708,7 +2779,7 @@
       <c r="K155" s="1"/>
       <c r="L155" s="1"/>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -2718,7 +2789,7 @@
       <c r="K156" s="1"/>
       <c r="L156" s="1"/>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -2728,7 +2799,7 @@
       <c r="K157" s="1"/>
       <c r="L157" s="1"/>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -2738,7 +2809,7 @@
       <c r="K158" s="1"/>
       <c r="L158" s="1"/>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -2748,7 +2819,7 @@
       <c r="K159" s="1"/>
       <c r="L159" s="1"/>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -2758,7 +2829,7 @@
       <c r="K160" s="1"/>
       <c r="L160" s="1"/>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -2768,7 +2839,7 @@
       <c r="K161" s="1"/>
       <c r="L161" s="1"/>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -2778,7 +2849,7 @@
       <c r="K162" s="1"/>
       <c r="L162" s="1"/>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -2788,7 +2859,7 @@
       <c r="K163" s="1"/>
       <c r="L163" s="1"/>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -2798,7 +2869,7 @@
       <c r="K164" s="1"/>
       <c r="L164" s="1"/>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -2808,7 +2879,7 @@
       <c r="K165" s="1"/>
       <c r="L165" s="1"/>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -2818,7 +2889,7 @@
       <c r="K166" s="1"/>
       <c r="L166" s="1"/>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -2828,7 +2899,7 @@
       <c r="K167" s="1"/>
       <c r="L167" s="1"/>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -2838,7 +2909,7 @@
       <c r="K168" s="1"/>
       <c r="L168" s="1"/>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -2848,7 +2919,7 @@
       <c r="K169" s="1"/>
       <c r="L169" s="1"/>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -2858,7 +2929,7 @@
       <c r="K170" s="1"/>
       <c r="L170" s="1"/>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -2868,7 +2939,7 @@
       <c r="K171" s="1"/>
       <c r="L171" s="1"/>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -2878,7 +2949,7 @@
       <c r="K172" s="1"/>
       <c r="L172" s="1"/>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -2888,7 +2959,7 @@
       <c r="K173" s="1"/>
       <c r="L173" s="1"/>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -2898,7 +2969,7 @@
       <c r="K174" s="1"/>
       <c r="L174" s="1"/>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -2908,7 +2979,7 @@
       <c r="K175" s="1"/>
       <c r="L175" s="1"/>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -2918,7 +2989,7 @@
       <c r="K176" s="1"/>
       <c r="L176" s="1"/>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -2928,7 +2999,7 @@
       <c r="K177" s="1"/>
       <c r="L177" s="1"/>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -2938,7 +3009,7 @@
       <c r="K178" s="1"/>
       <c r="L178" s="1"/>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -2948,7 +3019,7 @@
       <c r="K179" s="1"/>
       <c r="L179" s="1"/>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -2958,7 +3029,7 @@
       <c r="K180" s="1"/>
       <c r="L180" s="1"/>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -2968,7 +3039,7 @@
       <c r="K181" s="1"/>
       <c r="L181" s="1"/>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -2978,7 +3049,7 @@
       <c r="K182" s="1"/>
       <c r="L182" s="1"/>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -2988,7 +3059,7 @@
       <c r="K183" s="1"/>
       <c r="L183" s="1"/>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -2998,7 +3069,7 @@
       <c r="K184" s="1"/>
       <c r="L184" s="1"/>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -3008,7 +3079,7 @@
       <c r="K185" s="1"/>
       <c r="L185" s="1"/>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -3018,7 +3089,7 @@
       <c r="K186" s="1"/>
       <c r="L186" s="1"/>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -3028,7 +3099,7 @@
       <c r="K187" s="1"/>
       <c r="L187" s="1"/>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -3038,7 +3109,7 @@
       <c r="K188" s="1"/>
       <c r="L188" s="1"/>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -3048,7 +3119,7 @@
       <c r="K189" s="1"/>
       <c r="L189" s="1"/>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -3058,7 +3129,7 @@
       <c r="K190" s="1"/>
       <c r="L190" s="1"/>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -3068,7 +3139,7 @@
       <c r="K191" s="1"/>
       <c r="L191" s="1"/>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -3078,7 +3149,7 @@
       <c r="K192" s="1"/>
       <c r="L192" s="1"/>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -3088,7 +3159,7 @@
       <c r="K193" s="1"/>
       <c r="L193" s="1"/>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -3098,7 +3169,7 @@
       <c r="K194" s="1"/>
       <c r="L194" s="1"/>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -3112,13 +3183,12 @@
   <hyperlinks>
     <hyperlink ref="C22" r:id="rId1" location="pm2"/>
     <hyperlink ref="H23" r:id="rId2"/>
-    <hyperlink ref="H8" r:id="rId3"/>
-    <hyperlink ref="H35" r:id="rId4"/>
-    <hyperlink ref="H25" r:id="rId5"/>
-    <hyperlink ref="H31" r:id="rId6" display="https://www.rplumber.io/docs/index.html"/>
-    <hyperlink ref="H32" r:id="rId7"/>
+    <hyperlink ref="H35" r:id="rId3"/>
+    <hyperlink ref="H25" r:id="rId4"/>
+    <hyperlink ref="H31" r:id="rId5" display="https://www.rplumber.io/docs/index.html"/>
+    <hyperlink ref="H32" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="58" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
+  <pageSetup paperSize="9" scale="58" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Amazon AWL Link mit Infos zu R hinzugefügt
</commit_message>
<xml_diff>
--- a/tools.xlsx
+++ b/tools.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vepo\Documents\GitRepo\operationalisierung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soga\Documents\02_Projekte\00_Operationalisierung\operationalisierung\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="13248"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="13245"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="103">
   <si>
     <t>Name</t>
   </si>
@@ -211,9 +211,6 @@
   </si>
   <si>
     <t>Beschreibung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Docker provides a way to run applications securely isolated in a container, packaged with all its dependencies and libraries. </t>
   </si>
   <si>
     <t>https://docs.docker.com/</t>
@@ -359,6 +356,13 @@
   </si>
   <si>
     <t xml:space="preserve">Mehr ein Speichersystem. Es ist möglich über eine Docker Machine eine API Adresse mit Container zu kreieren. Dies benötigt aber Zugang zu anderem Tool z.B. DigitalOcean (siehe https://www.youtube.com/watch?v=jlVrYgVEl6M) </t>
+  </si>
+  <si>
+    <t>How to use AWS for R: 
+https://aws.amazon.com/de/blogs/big-data/running-r-on-aws/</t>
+  </si>
+  <si>
+    <t>Docker provides a way to run applications securely isolated in a container, packaged with all its dependencies and libraries. Eine Art lightweight Virtual Machine</t>
   </si>
 </sst>
 </file>
@@ -767,24 +771,24 @@
   <dimension ref="A1:L195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" style="1" customWidth="1"/>
-    <col min="7" max="8" width="45.5546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="37.44140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="45.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="37.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>46</v>
       </c>
@@ -793,7 +797,7 @@
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -804,13 +808,13 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>61</v>
@@ -825,9 +829,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="155.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>2</v>
@@ -836,28 +840,28 @@
         <v>42</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>84</v>
-      </c>
       <c r="I3" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -871,7 +875,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" s="14" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="14" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>27</v>
       </c>
@@ -882,7 +886,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
@@ -890,14 +894,14 @@
         <v>56</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
@@ -914,22 +918,22 @@
         <v>18</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G6" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="I6" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>94</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" s="14" customFormat="1" ht="118.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="14" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
@@ -940,28 +944,28 @@
         <v>8</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I7" s="12"/>
       <c r="J7" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12" ht="95.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="95.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
@@ -981,13 +985,13 @@
         <v>60</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>21</v>
       </c>
@@ -1007,7 +1011,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>6</v>
       </c>
@@ -1029,7 +1033,7 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="66" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
@@ -1040,24 +1044,24 @@
         <v>8</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>25</v>
       </c>
@@ -1075,7 +1079,9 @@
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="H12" s="8" t="s">
+        <v>101</v>
+      </c>
       <c r="I12" s="8" t="s">
         <v>33</v>
       </c>
@@ -1083,7 +1089,7 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>20</v>
       </c>
@@ -1101,7 +1107,7 @@
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
@@ -1109,7 +1115,7 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>34</v>
       </c>
@@ -1129,7 +1135,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
@@ -1153,7 +1159,7 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>31</v>
       </c>
@@ -1171,7 +1177,7 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1185,7 +1191,7 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -1199,7 +1205,7 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -1213,7 +1219,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -1227,7 +1233,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1241,7 +1247,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>37</v>
       </c>
@@ -1259,12 +1265,12 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8" t="s">
@@ -1287,7 +1293,7 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>41</v>
       </c>
@@ -1303,7 +1309,7 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>40</v>
       </c>
@@ -1313,27 +1319,27 @@
         <v>8</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G25" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H25" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H25" s="9" t="s">
-        <v>63</v>
-      </c>
       <c r="I25" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>49</v>
       </c>
@@ -1343,17 +1349,17 @@
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -1367,7 +1373,7 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -1381,7 +1387,7 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -1395,7 +1401,7 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>45</v>
       </c>
@@ -1413,7 +1419,7 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="1:12" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>10</v>
       </c>
@@ -1427,21 +1433,21 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>48</v>
       </c>
@@ -1456,16 +1462,16 @@
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J32" s="8"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>26</v>
       </c>
@@ -1491,7 +1497,7 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>50</v>
       </c>
@@ -1513,7 +1519,7 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
-    <row r="35" spans="1:12" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>29</v>
       </c>
@@ -1535,7 +1541,7 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -1549,7 +1555,7 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -1563,7 +1569,7 @@
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -1577,7 +1583,7 @@
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -1591,7 +1597,7 @@
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -1605,7 +1611,7 @@
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -1619,7 +1625,7 @@
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -1633,7 +1639,7 @@
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -1647,7 +1653,7 @@
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -1661,7 +1667,7 @@
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -1675,7 +1681,7 @@
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -1689,7 +1695,7 @@
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1699,7 +1705,7 @@
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1709,7 +1715,7 @@
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1719,7 +1725,7 @@
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1729,7 +1735,7 @@
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1739,7 +1745,7 @@
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1749,7 +1755,7 @@
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1759,7 +1765,7 @@
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1769,7 +1775,7 @@
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1779,7 +1785,7 @@
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1789,7 +1795,7 @@
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1799,7 +1805,7 @@
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1809,7 +1815,7 @@
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1819,7 +1825,7 @@
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1829,7 +1835,7 @@
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1839,7 +1845,7 @@
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1849,7 +1855,7 @@
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1859,7 +1865,7 @@
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1869,7 +1875,7 @@
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1879,7 +1885,7 @@
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1889,7 +1895,7 @@
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1899,7 +1905,7 @@
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1909,7 +1915,7 @@
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1919,7 +1925,7 @@
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1929,7 +1935,7 @@
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1939,7 +1945,7 @@
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1949,7 +1955,7 @@
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1959,7 +1965,7 @@
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1969,7 +1975,7 @@
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1979,7 +1985,7 @@
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1989,7 +1995,7 @@
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1999,7 +2005,7 @@
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2009,7 +2015,7 @@
       <c r="K78" s="1"/>
       <c r="L78" s="1"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2019,7 +2025,7 @@
       <c r="K79" s="1"/>
       <c r="L79" s="1"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2029,7 +2035,7 @@
       <c r="K80" s="1"/>
       <c r="L80" s="1"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2039,7 +2045,7 @@
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2049,7 +2055,7 @@
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2059,7 +2065,7 @@
       <c r="K83" s="1"/>
       <c r="L83" s="1"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2069,7 +2075,7 @@
       <c r="K84" s="1"/>
       <c r="L84" s="1"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2079,7 +2085,7 @@
       <c r="K85" s="1"/>
       <c r="L85" s="1"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2089,7 +2095,7 @@
       <c r="K86" s="1"/>
       <c r="L86" s="1"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2099,7 +2105,7 @@
       <c r="K87" s="1"/>
       <c r="L87" s="1"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2109,7 +2115,7 @@
       <c r="K88" s="1"/>
       <c r="L88" s="1"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2119,7 +2125,7 @@
       <c r="K89" s="1"/>
       <c r="L89" s="1"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2129,7 +2135,7 @@
       <c r="K90" s="1"/>
       <c r="L90" s="1"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2139,7 +2145,7 @@
       <c r="K91" s="1"/>
       <c r="L91" s="1"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2149,7 +2155,7 @@
       <c r="K92" s="1"/>
       <c r="L92" s="1"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2159,7 +2165,7 @@
       <c r="K93" s="1"/>
       <c r="L93" s="1"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2169,7 +2175,7 @@
       <c r="K94" s="1"/>
       <c r="L94" s="1"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2179,7 +2185,7 @@
       <c r="K95" s="1"/>
       <c r="L95" s="1"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2189,7 +2195,7 @@
       <c r="K96" s="1"/>
       <c r="L96" s="1"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2199,7 +2205,7 @@
       <c r="K97" s="1"/>
       <c r="L97" s="1"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2209,7 +2215,7 @@
       <c r="K98" s="1"/>
       <c r="L98" s="1"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2219,7 +2225,7 @@
       <c r="K99" s="1"/>
       <c r="L99" s="1"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2229,7 +2235,7 @@
       <c r="K100" s="1"/>
       <c r="L100" s="1"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -2239,7 +2245,7 @@
       <c r="K101" s="1"/>
       <c r="L101" s="1"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -2249,7 +2255,7 @@
       <c r="K102" s="1"/>
       <c r="L102" s="1"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2259,7 +2265,7 @@
       <c r="K103" s="1"/>
       <c r="L103" s="1"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -2269,7 +2275,7 @@
       <c r="K104" s="1"/>
       <c r="L104" s="1"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2279,7 +2285,7 @@
       <c r="K105" s="1"/>
       <c r="L105" s="1"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2289,7 +2295,7 @@
       <c r="K106" s="1"/>
       <c r="L106" s="1"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -2299,7 +2305,7 @@
       <c r="K107" s="1"/>
       <c r="L107" s="1"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -2309,7 +2315,7 @@
       <c r="K108" s="1"/>
       <c r="L108" s="1"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -2319,7 +2325,7 @@
       <c r="K109" s="1"/>
       <c r="L109" s="1"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -2329,7 +2335,7 @@
       <c r="K110" s="1"/>
       <c r="L110" s="1"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -2339,7 +2345,7 @@
       <c r="K111" s="1"/>
       <c r="L111" s="1"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -2349,7 +2355,7 @@
       <c r="K112" s="1"/>
       <c r="L112" s="1"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -2359,7 +2365,7 @@
       <c r="K113" s="1"/>
       <c r="L113" s="1"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -2369,7 +2375,7 @@
       <c r="K114" s="1"/>
       <c r="L114" s="1"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -2379,7 +2385,7 @@
       <c r="K115" s="1"/>
       <c r="L115" s="1"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -2389,7 +2395,7 @@
       <c r="K116" s="1"/>
       <c r="L116" s="1"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -2399,7 +2405,7 @@
       <c r="K117" s="1"/>
       <c r="L117" s="1"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -2409,7 +2415,7 @@
       <c r="K118" s="1"/>
       <c r="L118" s="1"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -2419,7 +2425,7 @@
       <c r="K119" s="1"/>
       <c r="L119" s="1"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -2429,7 +2435,7 @@
       <c r="K120" s="1"/>
       <c r="L120" s="1"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -2439,7 +2445,7 @@
       <c r="K121" s="1"/>
       <c r="L121" s="1"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -2449,7 +2455,7 @@
       <c r="K122" s="1"/>
       <c r="L122" s="1"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -2459,7 +2465,7 @@
       <c r="K123" s="1"/>
       <c r="L123" s="1"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -2469,7 +2475,7 @@
       <c r="K124" s="1"/>
       <c r="L124" s="1"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -2479,7 +2485,7 @@
       <c r="K125" s="1"/>
       <c r="L125" s="1"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -2489,7 +2495,7 @@
       <c r="K126" s="1"/>
       <c r="L126" s="1"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -2499,7 +2505,7 @@
       <c r="K127" s="1"/>
       <c r="L127" s="1"/>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -2509,7 +2515,7 @@
       <c r="K128" s="1"/>
       <c r="L128" s="1"/>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -2519,7 +2525,7 @@
       <c r="K129" s="1"/>
       <c r="L129" s="1"/>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -2529,7 +2535,7 @@
       <c r="K130" s="1"/>
       <c r="L130" s="1"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -2539,7 +2545,7 @@
       <c r="K131" s="1"/>
       <c r="L131" s="1"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -2549,7 +2555,7 @@
       <c r="K132" s="1"/>
       <c r="L132" s="1"/>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -2559,7 +2565,7 @@
       <c r="K133" s="1"/>
       <c r="L133" s="1"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -2569,7 +2575,7 @@
       <c r="K134" s="1"/>
       <c r="L134" s="1"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -2579,7 +2585,7 @@
       <c r="K135" s="1"/>
       <c r="L135" s="1"/>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -2589,7 +2595,7 @@
       <c r="K136" s="1"/>
       <c r="L136" s="1"/>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -2599,7 +2605,7 @@
       <c r="K137" s="1"/>
       <c r="L137" s="1"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -2609,7 +2615,7 @@
       <c r="K138" s="1"/>
       <c r="L138" s="1"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -2619,7 +2625,7 @@
       <c r="K139" s="1"/>
       <c r="L139" s="1"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -2629,7 +2635,7 @@
       <c r="K140" s="1"/>
       <c r="L140" s="1"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -2639,7 +2645,7 @@
       <c r="K141" s="1"/>
       <c r="L141" s="1"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -2649,7 +2655,7 @@
       <c r="K142" s="1"/>
       <c r="L142" s="1"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -2659,7 +2665,7 @@
       <c r="K143" s="1"/>
       <c r="L143" s="1"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -2669,7 +2675,7 @@
       <c r="K144" s="1"/>
       <c r="L144" s="1"/>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -2679,7 +2685,7 @@
       <c r="K145" s="1"/>
       <c r="L145" s="1"/>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -2689,7 +2695,7 @@
       <c r="K146" s="1"/>
       <c r="L146" s="1"/>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -2699,7 +2705,7 @@
       <c r="K147" s="1"/>
       <c r="L147" s="1"/>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -2709,7 +2715,7 @@
       <c r="K148" s="1"/>
       <c r="L148" s="1"/>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -2719,7 +2725,7 @@
       <c r="K149" s="1"/>
       <c r="L149" s="1"/>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -2729,7 +2735,7 @@
       <c r="K150" s="1"/>
       <c r="L150" s="1"/>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -2739,7 +2745,7 @@
       <c r="K151" s="1"/>
       <c r="L151" s="1"/>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -2749,7 +2755,7 @@
       <c r="K152" s="1"/>
       <c r="L152" s="1"/>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -2759,7 +2765,7 @@
       <c r="K153" s="1"/>
       <c r="L153" s="1"/>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -2769,7 +2775,7 @@
       <c r="K154" s="1"/>
       <c r="L154" s="1"/>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -2779,7 +2785,7 @@
       <c r="K155" s="1"/>
       <c r="L155" s="1"/>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -2789,7 +2795,7 @@
       <c r="K156" s="1"/>
       <c r="L156" s="1"/>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -2799,7 +2805,7 @@
       <c r="K157" s="1"/>
       <c r="L157" s="1"/>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -2809,7 +2815,7 @@
       <c r="K158" s="1"/>
       <c r="L158" s="1"/>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -2819,7 +2825,7 @@
       <c r="K159" s="1"/>
       <c r="L159" s="1"/>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -2829,7 +2835,7 @@
       <c r="K160" s="1"/>
       <c r="L160" s="1"/>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -2839,7 +2845,7 @@
       <c r="K161" s="1"/>
       <c r="L161" s="1"/>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -2849,7 +2855,7 @@
       <c r="K162" s="1"/>
       <c r="L162" s="1"/>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -2859,7 +2865,7 @@
       <c r="K163" s="1"/>
       <c r="L163" s="1"/>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -2869,7 +2875,7 @@
       <c r="K164" s="1"/>
       <c r="L164" s="1"/>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -2879,7 +2885,7 @@
       <c r="K165" s="1"/>
       <c r="L165" s="1"/>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -2889,7 +2895,7 @@
       <c r="K166" s="1"/>
       <c r="L166" s="1"/>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -2899,7 +2905,7 @@
       <c r="K167" s="1"/>
       <c r="L167" s="1"/>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -2909,7 +2915,7 @@
       <c r="K168" s="1"/>
       <c r="L168" s="1"/>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -2919,7 +2925,7 @@
       <c r="K169" s="1"/>
       <c r="L169" s="1"/>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -2929,7 +2935,7 @@
       <c r="K170" s="1"/>
       <c r="L170" s="1"/>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -2939,7 +2945,7 @@
       <c r="K171" s="1"/>
       <c r="L171" s="1"/>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -2949,7 +2955,7 @@
       <c r="K172" s="1"/>
       <c r="L172" s="1"/>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -2959,7 +2965,7 @@
       <c r="K173" s="1"/>
       <c r="L173" s="1"/>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -2969,7 +2975,7 @@
       <c r="K174" s="1"/>
       <c r="L174" s="1"/>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -2979,7 +2985,7 @@
       <c r="K175" s="1"/>
       <c r="L175" s="1"/>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -2989,7 +2995,7 @@
       <c r="K176" s="1"/>
       <c r="L176" s="1"/>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -2999,7 +3005,7 @@
       <c r="K177" s="1"/>
       <c r="L177" s="1"/>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -3009,7 +3015,7 @@
       <c r="K178" s="1"/>
       <c r="L178" s="1"/>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -3019,7 +3025,7 @@
       <c r="K179" s="1"/>
       <c r="L179" s="1"/>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -3029,7 +3035,7 @@
       <c r="K180" s="1"/>
       <c r="L180" s="1"/>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -3039,7 +3045,7 @@
       <c r="K181" s="1"/>
       <c r="L181" s="1"/>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -3049,7 +3055,7 @@
       <c r="K182" s="1"/>
       <c r="L182" s="1"/>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -3059,7 +3065,7 @@
       <c r="K183" s="1"/>
       <c r="L183" s="1"/>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -3069,7 +3075,7 @@
       <c r="K184" s="1"/>
       <c r="L184" s="1"/>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -3079,7 +3085,7 @@
       <c r="K185" s="1"/>
       <c r="L185" s="1"/>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -3089,7 +3095,7 @@
       <c r="K186" s="1"/>
       <c r="L186" s="1"/>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -3099,7 +3105,7 @@
       <c r="K187" s="1"/>
       <c r="L187" s="1"/>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -3109,7 +3115,7 @@
       <c r="K188" s="1"/>
       <c r="L188" s="1"/>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -3119,7 +3125,7 @@
       <c r="K189" s="1"/>
       <c r="L189" s="1"/>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -3129,7 +3135,7 @@
       <c r="K190" s="1"/>
       <c r="L190" s="1"/>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -3139,7 +3145,7 @@
       <c r="K191" s="1"/>
       <c r="L191" s="1"/>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -3149,7 +3155,7 @@
       <c r="K192" s="1"/>
       <c r="L192" s="1"/>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -3159,7 +3165,7 @@
       <c r="K193" s="1"/>
       <c r="L193" s="1"/>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -3169,7 +3175,7 @@
       <c r="K194" s="1"/>
       <c r="L194" s="1"/>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>

</xml_diff>

<commit_message>
updated .gitignore to not track any files named old...
</commit_message>
<xml_diff>
--- a/tools.xlsx
+++ b/tools.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -77,18 +77,12 @@
     <t>R Package</t>
   </si>
   <si>
-    <t>1 Jahr</t>
-  </si>
-  <si>
     <t>45 Tage</t>
   </si>
   <si>
     <t>14 Tage</t>
   </si>
   <si>
-    <t>SparkR (amazon)</t>
-  </si>
-  <si>
     <t>SAP HANA</t>
   </si>
   <si>
@@ -107,9 +101,6 @@
     <t>sparklyr</t>
   </si>
   <si>
-    <t>Microsoft DeployR</t>
-  </si>
-  <si>
     <t>Serialisierung (ist R Package)</t>
   </si>
   <si>
@@ -137,19 +128,10 @@
     <t>Installation</t>
   </si>
   <si>
-    <t>Vorschläge von plumber-Dokumentation (Chapter 7: Hosting)</t>
-  </si>
-  <si>
-    <t>https://www.rplumber.io/docs/hosting.html#pm2</t>
-  </si>
-  <si>
     <t>DigitalOcean</t>
   </si>
   <si>
     <t>Docker</t>
-  </si>
-  <si>
-    <t>Rstudio Connect (siehe oben)</t>
   </si>
   <si>
     <t>ja</t>
@@ -323,9 +305,6 @@
     <t>free available</t>
   </si>
   <si>
-    <t>Verbindung zwischen R und Spark.</t>
-  </si>
-  <si>
     <t>RStudio Connect is a new publishing platform for the work your teams create in R. Share Shiny applications, R Markdown reports, dashboards, plots, and more in one convenient place. Use push-button publishing from the RStudio IDE, scheduled execution of reports, and flexible security policies to bring the power of data science to your entire enterprise.</t>
   </si>
   <si>
@@ -362,14 +341,29 @@
 https://aws.amazon.com/de/blogs/big-data/running-r-on-aws/</t>
   </si>
   <si>
-    <t>Docker provides a way to run applications securely isolated in a container, packaged with all its dependencies and libraries. Eine Art lightweight Virtual Machine</t>
+    <t>(Microsoft DeployR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">veraltet: Formerly known as DeployR, this capability for operationalizing your code is fully integrated into R Server resp. MS ML Server. </t>
+  </si>
+  <si>
+    <t>Veraltet</t>
+  </si>
+  <si>
+    <t>Out of Scope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eine Art lightweight Virtual Machine. Docker provides a way to run applications securely isolated in a container, packaged with all its dependencies and libraries. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rserve ist gemäss Gian-Marco in SAP HANA integriert, somit lohnt es sich nicht SAP HANA anzuschauen. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -390,13 +384,6 @@
       <color theme="10"/>
       <name val="AA Zuehlke"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="AA Zuehlke"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -440,7 +427,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -452,9 +439,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -464,9 +451,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -768,11 +752,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L195"/>
+  <dimension ref="A1:L192"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -790,7 +774,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
@@ -808,169 +792,181 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="155.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
+      <c r="H4" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="J4" s="8"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" s="14" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="12" t="s">
+    <row r="5" spans="1:12" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-    </row>
-    <row r="6" spans="1:12" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="D5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" s="8"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" s="13" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+    </row>
+    <row r="7" spans="1:12" ht="135" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="J6" s="8"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" s="14" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-    </row>
-    <row r="8" spans="1:12" ht="95.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" s="8"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>8</v>
@@ -978,14 +974,10 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="H8" t="s">
-        <v>60</v>
-      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
       <c r="I8" s="8" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="1"/>
@@ -993,7 +985,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>7</v>
@@ -1006,14 +998,16 @@
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="I9" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="J9" s="8"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>7</v>
@@ -1021,69 +1015,39 @@
       <c r="C10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="8" t="s">
+        <v>73</v>
+      </c>
       <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>75</v>
+      </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>7</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="8" t="s">
-        <v>101</v>
-      </c>
+      <c r="H12" s="8"/>
       <c r="I12" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="1"/>
@@ -1091,11 +1055,9 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>7</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1103,66 +1065,52 @@
         <v>8</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F13" s="8"/>
-      <c r="G13" s="8" t="s">
-        <v>90</v>
-      </c>
+      <c r="G13" s="8"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
+      <c r="I13" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="J13" s="8"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B14" s="8"/>
-      <c r="C14" s="8" t="s">
-        <v>8</v>
-      </c>
+      <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="A15" s="8"/>
       <c r="B15" s="8"/>
-      <c r="C15" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>19</v>
-      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
-      <c r="I15" s="8" t="s">
-        <v>22</v>
-      </c>
+      <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
-        <v>31</v>
-      </c>
+      <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -1170,9 +1118,7 @@
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="8" t="s">
-        <v>32</v>
-      </c>
+      <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1219,15 +1165,29 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
+    <row r="20" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
+      <c r="D20" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
       <c r="K20" s="1"/>
@@ -1247,56 +1207,8 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-    </row>
-    <row r="23" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-    </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -1309,59 +1221,41 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="8" t="s">
-        <v>40</v>
-      </c>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>99</v>
-      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A26" s="8" t="s">
-        <v>49</v>
-      </c>
+    <row r="26" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
-      <c r="G26" s="8" t="s">
-        <v>63</v>
-      </c>
+      <c r="G26" s="8"/>
       <c r="H26" s="8"/>
-      <c r="I26" s="8" t="s">
-        <v>64</v>
-      </c>
+      <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
+    <row r="27" spans="1:12" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -1373,55 +1267,87 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
+    <row r="28" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
+      <c r="G28" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>91</v>
+      </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
+    <row r="29" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
+      <c r="H29" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="J29" s="8"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
-        <v>45</v>
+    <row r="30" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
+      <c r="G30" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
+      <c r="I30" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="J30" s="8"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>16</v>
@@ -1433,26 +1359,20 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>98</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>8</v>
@@ -1462,80 +1382,50 @@
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
       <c r="H32" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>67</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>8</v>
-      </c>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
-      <c r="G33" s="8" t="s">
-        <v>53</v>
-      </c>
+      <c r="G33" s="8"/>
       <c r="H33" s="8"/>
-      <c r="I33" s="8" t="s">
-        <v>51</v>
-      </c>
+      <c r="I33" s="8"/>
       <c r="J33" s="8"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>8</v>
-      </c>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
-      <c r="G34" s="8" t="s">
-        <v>52</v>
-      </c>
+      <c r="G34" s="8"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
-    <row r="35" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>8</v>
-      </c>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
-      <c r="H35" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="H35" s="8"/>
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
       <c r="K35" s="1"/>
@@ -1555,8 +1445,10 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="8"/>
+    <row r="37" spans="1:12" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>97</v>
+      </c>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
@@ -1569,19 +1461,33 @@
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
+    <row r="38" spans="1:12" s="13" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="J38" s="11"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="8"/>
@@ -1625,8 +1531,10 @@
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="8"/>
+    <row r="42" spans="1:12" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="10" t="s">
+        <v>98</v>
+      </c>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
@@ -1639,8 +1547,10 @@
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="8"/>
+    <row r="43" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
@@ -1653,45 +1563,63 @@
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" s="8"/>
+    <row r="44" spans="1:12" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
+      <c r="D44" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="J44" s="8" t="s">
+        <v>92</v>
+      </c>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" s="8"/>
+    <row r="45" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A45" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
+      <c r="G45" s="8" t="s">
+        <v>57</v>
+      </c>
       <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
+      <c r="I45" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="J45" s="8"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
     </row>
@@ -3155,46 +3083,15 @@
       <c r="K192" s="1"/>
       <c r="L192" s="1"/>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A193" s="1"/>
-      <c r="B193" s="1"/>
-      <c r="C193" s="1"/>
-      <c r="D193" s="1"/>
-      <c r="E193" s="1"/>
-      <c r="J193" s="1"/>
-      <c r="K193" s="1"/>
-      <c r="L193" s="1"/>
-    </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A194" s="1"/>
-      <c r="B194" s="1"/>
-      <c r="C194" s="1"/>
-      <c r="D194" s="1"/>
-      <c r="E194" s="1"/>
-      <c r="J194" s="1"/>
-      <c r="K194" s="1"/>
-      <c r="L194" s="1"/>
-    </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A195" s="1"/>
-      <c r="B195" s="1"/>
-      <c r="C195" s="1"/>
-      <c r="D195" s="1"/>
-      <c r="E195" s="1"/>
-      <c r="J195" s="1"/>
-      <c r="K195" s="1"/>
-      <c r="L195" s="1"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C22" r:id="rId1" location="pm2"/>
-    <hyperlink ref="H23" r:id="rId2"/>
-    <hyperlink ref="H35" r:id="rId3"/>
-    <hyperlink ref="H25" r:id="rId4"/>
-    <hyperlink ref="H31" r:id="rId5" display="https://www.rplumber.io/docs/index.html"/>
-    <hyperlink ref="H32" r:id="rId6"/>
+    <hyperlink ref="H20" r:id="rId1"/>
+    <hyperlink ref="H32" r:id="rId2"/>
+    <hyperlink ref="H44" r:id="rId3"/>
+    <hyperlink ref="H28" r:id="rId4" display="https://www.rplumber.io/docs/index.html"/>
+    <hyperlink ref="H29" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="58" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
+  <pageSetup paperSize="9" scale="58" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Beschreibung zu MS ML Server updated
</commit_message>
<xml_diff>
--- a/tools.xlsx
+++ b/tools.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="13245"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="13248"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="102">
   <si>
     <t>Name</t>
   </si>
@@ -279,10 +279,6 @@
     <t>Commercial Tool for doing machine learning and operationalize your solution</t>
   </si>
   <si>
-    <t>Namen ist verwirrend: MS R Server ist kein Server, sondern ein Framework, um auf einem (bestehenden) Server oder auf einer Cloud (z.B. von MS Azure) R-Skripte laufen zu lassen. Beinhaltet R-distribution (MS R Open), welche bestimmte MS packages enthält, welche Deployment und Parallelisierung auf Server oder Cloud, auf welcher MS R Server installiert ist, zulassen. (mrsdeploy, RevoScaleR)
-R and Python code and models can be deployed as web services. Exposed as web services hosted in Machine Learning Server, these models and code can be accessed and consumed in R, Python, programmatically using REST APIs, or using Swagger generated client libraries. Web services can be deployed from one platform and consumed on another. They can be consumed synchronously, in realtime, or in batch mode.</t>
-  </si>
-  <si>
     <t>https://docs.microsoft.com/en-us/machine-learning-server/
 https://docs.microsoft.com/en-us/machine-learning-server/operationalize/concept-what-are-web-services</t>
   </si>
@@ -357,13 +353,43 @@
   </si>
   <si>
     <t xml:space="preserve">Rserve ist gemäss Gian-Marco in SAP HANA integriert, somit lohnt es sich nicht SAP HANA anzuschauen. </t>
+  </si>
+  <si>
+    <t>R Solution</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Details siehe File </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="AA Zuehlke"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MS-R-Server_und_ML-Server</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="AA Zuehlke"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+--
+Namen ist verwirrend: MS R Server ist kein Server, sondern ein Framework, um auf einem (bestehenden) Server oder auf einer Cloud (z.B. von MS Azure) R-Skripte laufen zu lassen. Beinhaltet R-distribution (MS R Open), welche bestimmte MS packages enthält, welche Deployment und Parallelisierung auf Server oder Cloud, auf welcher MS R Server installiert ist, zulassen. (mrsdeploy, RevoScaleR)
+R and Python code and models can be deployed as web services. Exposed as web services hosted in Machine Learning Server, these models and code can be accessed and consumed in R, Python, programmatically using REST APIs, or using Swagger generated client libraries. Web services can be deployed from one platform and consumed on another. They can be consumed synchronously, in realtime, or in batch mode.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -403,6 +429,12 @@
       <color theme="10"/>
       <name val="AA Zuehlke"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="AA Zuehlke"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -756,23 +788,23 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="45.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="37.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.71875" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="22.27734375" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="6" max="6" width="28.27734375" style="1" customWidth="1"/>
+    <col min="7" max="8" width="45.5546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="37.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.27734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="6" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.7">
       <c r="A1" s="5" t="s">
         <v>40</v>
       </c>
@@ -781,7 +813,7 @@
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -813,12 +845,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="155.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="155.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
         <v>67</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>36</v>
@@ -831,10 +863,10 @@
         <v>15</v>
       </c>
       <c r="G3" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>77</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>65</v>
@@ -843,7 +875,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="37.799999999999997" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>23</v>
       </c>
@@ -862,7 +894,7 @@
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>30</v>
@@ -871,7 +903,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="88.2" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -888,22 +920,22 @@
         <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G5" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="I5" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>86</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" s="13" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" s="13" customFormat="1" ht="113.4" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
@@ -914,28 +946,28 @@
         <v>8</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" ht="135" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="135" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -961,7 +993,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="37.799999999999997" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
         <v>19</v>
       </c>
@@ -977,13 +1009,13 @@
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
         <v>6</v>
       </c>
@@ -1005,7 +1037,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="63" x14ac:dyDescent="0.45">
       <c r="A10" s="8" t="s">
         <v>13</v>
       </c>
@@ -1033,7 +1065,7 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="25.2" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
         <v>31</v>
       </c>
@@ -1053,7 +1085,7 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
@@ -1077,7 +1109,7 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="8" t="s">
         <v>28</v>
       </c>
@@ -1095,7 +1127,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -1109,7 +1141,7 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1123,7 +1155,7 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1137,7 +1169,7 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -1151,7 +1183,7 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -1165,12 +1197,12 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8" t="s">
@@ -1193,7 +1225,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -1207,7 +1239,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -1221,7 +1253,7 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -1235,7 +1267,7 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1249,7 +1281,7 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A27" s="10" t="s">
         <v>39</v>
       </c>
@@ -1267,7 +1299,7 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="50.4" x14ac:dyDescent="0.45">
       <c r="A28" s="8" t="s">
         <v>10</v>
       </c>
@@ -1287,15 +1319,15 @@
         <v>63</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="8" t="s">
         <v>42</v>
       </c>
@@ -1319,7 +1351,7 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="8" t="s">
         <v>24</v>
       </c>
@@ -1345,7 +1377,7 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="25.2" x14ac:dyDescent="0.45">
       <c r="A31" s="8" t="s">
         <v>44</v>
       </c>
@@ -1367,7 +1399,7 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="25.2" x14ac:dyDescent="0.45">
       <c r="A32" s="8" t="s">
         <v>26</v>
       </c>
@@ -1389,7 +1421,7 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -1403,7 +1435,7 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -1417,7 +1449,7 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -1431,7 +1463,7 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -1445,9 +1477,9 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
     </row>
-    <row r="37" spans="1:12" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A37" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -1461,9 +1493,9 @@
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
     </row>
-    <row r="38" spans="1:12" s="13" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" s="13" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>2</v>
@@ -1483,13 +1515,13 @@
         <v>64</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J38" s="11"/>
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -1503,7 +1535,7 @@
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -1517,7 +1549,7 @@
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -1531,9 +1563,9 @@
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
     </row>
-    <row r="42" spans="1:12" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A42" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -1547,7 +1579,7 @@
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
     </row>
-    <row r="43" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="8" t="s">
         <v>66</v>
       </c>
@@ -1563,7 +1595,7 @@
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
     </row>
-    <row r="44" spans="1:12" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="75.599999999999994" x14ac:dyDescent="0.45">
       <c r="A44" s="8" t="s">
         <v>35</v>
       </c>
@@ -1573,27 +1605,27 @@
         <v>8</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H44" s="9" t="s">
         <v>56</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J44" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
     </row>
-    <row r="45" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="50.4" x14ac:dyDescent="0.45">
       <c r="A45" s="8" t="s">
         <v>43</v>
       </c>
@@ -1613,7 +1645,7 @@
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1623,7 +1655,7 @@
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1633,7 +1665,7 @@
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1643,7 +1675,7 @@
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1653,7 +1685,7 @@
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1663,7 +1695,7 @@
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1673,7 +1705,7 @@
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1683,7 +1715,7 @@
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1693,7 +1725,7 @@
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1703,7 +1735,7 @@
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1713,7 +1745,7 @@
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1723,7 +1755,7 @@
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1733,7 +1765,7 @@
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1743,7 +1775,7 @@
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1753,7 +1785,7 @@
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1763,7 +1795,7 @@
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1773,7 +1805,7 @@
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1783,7 +1815,7 @@
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1793,7 +1825,7 @@
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1803,7 +1835,7 @@
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1813,7 +1845,7 @@
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1823,7 +1855,7 @@
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1833,7 +1865,7 @@
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1843,7 +1875,7 @@
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1853,7 +1885,7 @@
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1863,7 +1895,7 @@
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1873,7 +1905,7 @@
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1883,7 +1915,7 @@
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1893,7 +1925,7 @@
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1903,7 +1935,7 @@
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1913,7 +1945,7 @@
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1923,7 +1955,7 @@
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1933,7 +1965,7 @@
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1943,7 +1975,7 @@
       <c r="K78" s="1"/>
       <c r="L78" s="1"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -1953,7 +1985,7 @@
       <c r="K79" s="1"/>
       <c r="L79" s="1"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -1963,7 +1995,7 @@
       <c r="K80" s="1"/>
       <c r="L80" s="1"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -1973,7 +2005,7 @@
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -1983,7 +2015,7 @@
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -1993,7 +2025,7 @@
       <c r="K83" s="1"/>
       <c r="L83" s="1"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2003,7 +2035,7 @@
       <c r="K84" s="1"/>
       <c r="L84" s="1"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2013,7 +2045,7 @@
       <c r="K85" s="1"/>
       <c r="L85" s="1"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2023,7 +2055,7 @@
       <c r="K86" s="1"/>
       <c r="L86" s="1"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2033,7 +2065,7 @@
       <c r="K87" s="1"/>
       <c r="L87" s="1"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2043,7 +2075,7 @@
       <c r="K88" s="1"/>
       <c r="L88" s="1"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2053,7 +2085,7 @@
       <c r="K89" s="1"/>
       <c r="L89" s="1"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2063,7 +2095,7 @@
       <c r="K90" s="1"/>
       <c r="L90" s="1"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2073,7 +2105,7 @@
       <c r="K91" s="1"/>
       <c r="L91" s="1"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2083,7 +2115,7 @@
       <c r="K92" s="1"/>
       <c r="L92" s="1"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2093,7 +2125,7 @@
       <c r="K93" s="1"/>
       <c r="L93" s="1"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2103,7 +2135,7 @@
       <c r="K94" s="1"/>
       <c r="L94" s="1"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2113,7 +2145,7 @@
       <c r="K95" s="1"/>
       <c r="L95" s="1"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2123,7 +2155,7 @@
       <c r="K96" s="1"/>
       <c r="L96" s="1"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2133,7 +2165,7 @@
       <c r="K97" s="1"/>
       <c r="L97" s="1"/>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2143,7 +2175,7 @@
       <c r="K98" s="1"/>
       <c r="L98" s="1"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2153,7 +2185,7 @@
       <c r="K99" s="1"/>
       <c r="L99" s="1"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2163,7 +2195,7 @@
       <c r="K100" s="1"/>
       <c r="L100" s="1"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -2173,7 +2205,7 @@
       <c r="K101" s="1"/>
       <c r="L101" s="1"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -2183,7 +2215,7 @@
       <c r="K102" s="1"/>
       <c r="L102" s="1"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2193,7 +2225,7 @@
       <c r="K103" s="1"/>
       <c r="L103" s="1"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -2203,7 +2235,7 @@
       <c r="K104" s="1"/>
       <c r="L104" s="1"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2213,7 +2245,7 @@
       <c r="K105" s="1"/>
       <c r="L105" s="1"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2223,7 +2255,7 @@
       <c r="K106" s="1"/>
       <c r="L106" s="1"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -2233,7 +2265,7 @@
       <c r="K107" s="1"/>
       <c r="L107" s="1"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -2243,7 +2275,7 @@
       <c r="K108" s="1"/>
       <c r="L108" s="1"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -2253,7 +2285,7 @@
       <c r="K109" s="1"/>
       <c r="L109" s="1"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -2263,7 +2295,7 @@
       <c r="K110" s="1"/>
       <c r="L110" s="1"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -2273,7 +2305,7 @@
       <c r="K111" s="1"/>
       <c r="L111" s="1"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -2283,7 +2315,7 @@
       <c r="K112" s="1"/>
       <c r="L112" s="1"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -2293,7 +2325,7 @@
       <c r="K113" s="1"/>
       <c r="L113" s="1"/>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -2303,7 +2335,7 @@
       <c r="K114" s="1"/>
       <c r="L114" s="1"/>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -2313,7 +2345,7 @@
       <c r="K115" s="1"/>
       <c r="L115" s="1"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -2323,7 +2355,7 @@
       <c r="K116" s="1"/>
       <c r="L116" s="1"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -2333,7 +2365,7 @@
       <c r="K117" s="1"/>
       <c r="L117" s="1"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -2343,7 +2375,7 @@
       <c r="K118" s="1"/>
       <c r="L118" s="1"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -2353,7 +2385,7 @@
       <c r="K119" s="1"/>
       <c r="L119" s="1"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -2363,7 +2395,7 @@
       <c r="K120" s="1"/>
       <c r="L120" s="1"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -2373,7 +2405,7 @@
       <c r="K121" s="1"/>
       <c r="L121" s="1"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -2383,7 +2415,7 @@
       <c r="K122" s="1"/>
       <c r="L122" s="1"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -2393,7 +2425,7 @@
       <c r="K123" s="1"/>
       <c r="L123" s="1"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -2403,7 +2435,7 @@
       <c r="K124" s="1"/>
       <c r="L124" s="1"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -2413,7 +2445,7 @@
       <c r="K125" s="1"/>
       <c r="L125" s="1"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -2423,7 +2455,7 @@
       <c r="K126" s="1"/>
       <c r="L126" s="1"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -2433,7 +2465,7 @@
       <c r="K127" s="1"/>
       <c r="L127" s="1"/>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -2443,7 +2475,7 @@
       <c r="K128" s="1"/>
       <c r="L128" s="1"/>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -2453,7 +2485,7 @@
       <c r="K129" s="1"/>
       <c r="L129" s="1"/>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -2463,7 +2495,7 @@
       <c r="K130" s="1"/>
       <c r="L130" s="1"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -2473,7 +2505,7 @@
       <c r="K131" s="1"/>
       <c r="L131" s="1"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -2483,7 +2515,7 @@
       <c r="K132" s="1"/>
       <c r="L132" s="1"/>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -2493,7 +2525,7 @@
       <c r="K133" s="1"/>
       <c r="L133" s="1"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -2503,7 +2535,7 @@
       <c r="K134" s="1"/>
       <c r="L134" s="1"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -2513,7 +2545,7 @@
       <c r="K135" s="1"/>
       <c r="L135" s="1"/>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -2523,7 +2555,7 @@
       <c r="K136" s="1"/>
       <c r="L136" s="1"/>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -2533,7 +2565,7 @@
       <c r="K137" s="1"/>
       <c r="L137" s="1"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -2543,7 +2575,7 @@
       <c r="K138" s="1"/>
       <c r="L138" s="1"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -2553,7 +2585,7 @@
       <c r="K139" s="1"/>
       <c r="L139" s="1"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -2563,7 +2595,7 @@
       <c r="K140" s="1"/>
       <c r="L140" s="1"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -2573,7 +2605,7 @@
       <c r="K141" s="1"/>
       <c r="L141" s="1"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -2583,7 +2615,7 @@
       <c r="K142" s="1"/>
       <c r="L142" s="1"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -2593,7 +2625,7 @@
       <c r="K143" s="1"/>
       <c r="L143" s="1"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -2603,7 +2635,7 @@
       <c r="K144" s="1"/>
       <c r="L144" s="1"/>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -2613,7 +2645,7 @@
       <c r="K145" s="1"/>
       <c r="L145" s="1"/>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -2623,7 +2655,7 @@
       <c r="K146" s="1"/>
       <c r="L146" s="1"/>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -2633,7 +2665,7 @@
       <c r="K147" s="1"/>
       <c r="L147" s="1"/>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -2643,7 +2675,7 @@
       <c r="K148" s="1"/>
       <c r="L148" s="1"/>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -2653,7 +2685,7 @@
       <c r="K149" s="1"/>
       <c r="L149" s="1"/>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -2663,7 +2695,7 @@
       <c r="K150" s="1"/>
       <c r="L150" s="1"/>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -2673,7 +2705,7 @@
       <c r="K151" s="1"/>
       <c r="L151" s="1"/>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -2683,7 +2715,7 @@
       <c r="K152" s="1"/>
       <c r="L152" s="1"/>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -2693,7 +2725,7 @@
       <c r="K153" s="1"/>
       <c r="L153" s="1"/>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -2703,7 +2735,7 @@
       <c r="K154" s="1"/>
       <c r="L154" s="1"/>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -2713,7 +2745,7 @@
       <c r="K155" s="1"/>
       <c r="L155" s="1"/>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -2723,7 +2755,7 @@
       <c r="K156" s="1"/>
       <c r="L156" s="1"/>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -2733,7 +2765,7 @@
       <c r="K157" s="1"/>
       <c r="L157" s="1"/>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -2743,7 +2775,7 @@
       <c r="K158" s="1"/>
       <c r="L158" s="1"/>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -2753,7 +2785,7 @@
       <c r="K159" s="1"/>
       <c r="L159" s="1"/>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -2763,7 +2795,7 @@
       <c r="K160" s="1"/>
       <c r="L160" s="1"/>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -2773,7 +2805,7 @@
       <c r="K161" s="1"/>
       <c r="L161" s="1"/>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -2783,7 +2815,7 @@
       <c r="K162" s="1"/>
       <c r="L162" s="1"/>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -2793,7 +2825,7 @@
       <c r="K163" s="1"/>
       <c r="L163" s="1"/>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -2803,7 +2835,7 @@
       <c r="K164" s="1"/>
       <c r="L164" s="1"/>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -2813,7 +2845,7 @@
       <c r="K165" s="1"/>
       <c r="L165" s="1"/>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -2823,7 +2855,7 @@
       <c r="K166" s="1"/>
       <c r="L166" s="1"/>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -2833,7 +2865,7 @@
       <c r="K167" s="1"/>
       <c r="L167" s="1"/>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -2843,7 +2875,7 @@
       <c r="K168" s="1"/>
       <c r="L168" s="1"/>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -2853,7 +2885,7 @@
       <c r="K169" s="1"/>
       <c r="L169" s="1"/>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -2863,7 +2895,7 @@
       <c r="K170" s="1"/>
       <c r="L170" s="1"/>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -2873,7 +2905,7 @@
       <c r="K171" s="1"/>
       <c r="L171" s="1"/>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -2883,7 +2915,7 @@
       <c r="K172" s="1"/>
       <c r="L172" s="1"/>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -2893,7 +2925,7 @@
       <c r="K173" s="1"/>
       <c r="L173" s="1"/>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -2903,7 +2935,7 @@
       <c r="K174" s="1"/>
       <c r="L174" s="1"/>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -2913,7 +2945,7 @@
       <c r="K175" s="1"/>
       <c r="L175" s="1"/>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -2923,7 +2955,7 @@
       <c r="K176" s="1"/>
       <c r="L176" s="1"/>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -2933,7 +2965,7 @@
       <c r="K177" s="1"/>
       <c r="L177" s="1"/>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -2943,7 +2975,7 @@
       <c r="K178" s="1"/>
       <c r="L178" s="1"/>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -2953,7 +2985,7 @@
       <c r="K179" s="1"/>
       <c r="L179" s="1"/>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -2963,7 +2995,7 @@
       <c r="K180" s="1"/>
       <c r="L180" s="1"/>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -2973,7 +3005,7 @@
       <c r="K181" s="1"/>
       <c r="L181" s="1"/>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -2983,7 +3015,7 @@
       <c r="K182" s="1"/>
       <c r="L182" s="1"/>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -2993,7 +3025,7 @@
       <c r="K183" s="1"/>
       <c r="L183" s="1"/>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -3003,7 +3035,7 @@
       <c r="K184" s="1"/>
       <c r="L184" s="1"/>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -3013,7 +3045,7 @@
       <c r="K185" s="1"/>
       <c r="L185" s="1"/>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -3023,7 +3055,7 @@
       <c r="K186" s="1"/>
       <c r="L186" s="1"/>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -3033,7 +3065,7 @@
       <c r="K187" s="1"/>
       <c r="L187" s="1"/>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -3043,7 +3075,7 @@
       <c r="K188" s="1"/>
       <c r="L188" s="1"/>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -3053,7 +3085,7 @@
       <c r="K189" s="1"/>
       <c r="L189" s="1"/>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -3063,7 +3095,7 @@
       <c r="K190" s="1"/>
       <c r="L190" s="1"/>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -3073,7 +3105,7 @@
       <c r="K191" s="1"/>
       <c r="L191" s="1"/>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>

</xml_diff>